<commit_message>
Codigo mejorado. Se agrega el workflow del paper linear modelling. Base de datos corregida: esfuerzo 2021.
</commit_message>
<xml_diff>
--- a/data/eventosgatosB18-21.xlsx
+++ b/data/eventosgatosB18-21.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="15360" windowHeight="7350"/>
+    <workbookView xWindow="0" yWindow="2400" windowWidth="15360" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="eventosgatos18-21" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="110">
   <si>
     <t>zona</t>
   </si>
@@ -66,21 +66,6 @@
     <t>118.70</t>
   </si>
   <si>
-    <t>alta</t>
-  </si>
-  <si>
-    <t>116.53</t>
-  </si>
-  <si>
-    <t>E03</t>
-  </si>
-  <si>
-    <t>Camping Solis</t>
-  </si>
-  <si>
-    <t>119.58</t>
-  </si>
-  <si>
     <t>112.14</t>
   </si>
   <si>
@@ -93,21 +78,6 @@
     <t>118.89</t>
   </si>
   <si>
-    <t>111.53</t>
-  </si>
-  <si>
-    <t>E05</t>
-  </si>
-  <si>
-    <t>Caballeriza</t>
-  </si>
-  <si>
-    <t>118.49</t>
-  </si>
-  <si>
-    <t>Caballeriza b</t>
-  </si>
-  <si>
     <t>115.11</t>
   </si>
   <si>
@@ -123,42 +93,12 @@
     <t>Basural</t>
   </si>
   <si>
-    <t>108.86</t>
-  </si>
-  <si>
-    <t>E07</t>
-  </si>
-  <si>
-    <t>Local Urbano</t>
-  </si>
-  <si>
-    <t>119.25</t>
-  </si>
-  <si>
     <t>118.38</t>
   </si>
   <si>
-    <t>E08</t>
-  </si>
-  <si>
-    <t>Jardin Alcides</t>
-  </si>
-  <si>
     <t>119.56</t>
   </si>
   <si>
-    <t>113.51</t>
-  </si>
-  <si>
-    <t>E09</t>
-  </si>
-  <si>
-    <t>CANE</t>
-  </si>
-  <si>
-    <t>115.26</t>
-  </si>
-  <si>
     <t>119.02</t>
   </si>
   <si>
@@ -171,30 +111,6 @@
     <t>119.67</t>
   </si>
   <si>
-    <t>118.54</t>
-  </si>
-  <si>
-    <t>E11</t>
-  </si>
-  <si>
-    <t>Usina</t>
-  </si>
-  <si>
-    <t>121.4</t>
-  </si>
-  <si>
-    <t>115.98</t>
-  </si>
-  <si>
-    <t>E12</t>
-  </si>
-  <si>
-    <t>Club Brisas</t>
-  </si>
-  <si>
-    <t>119.35</t>
-  </si>
-  <si>
     <t>118.36</t>
   </si>
   <si>
@@ -427,27 +343,6 @@
   </si>
   <si>
     <t>120.07</t>
-  </si>
-  <si>
-    <t>117.98</t>
-  </si>
-  <si>
-    <t>E33</t>
-  </si>
-  <si>
-    <t>Fragata</t>
-  </si>
-  <si>
-    <t>118.78</t>
-  </si>
-  <si>
-    <t>E34</t>
-  </si>
-  <si>
-    <t>Museo</t>
-  </si>
-  <si>
-    <t>119.81</t>
   </si>
   <si>
     <t>esfuerzo</t>
@@ -937,8 +832,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1260,10 +1156,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H77"/>
+  <dimension ref="A1:H59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,13 +1170,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>144</v>
+        <v>109</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>108</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1430,74 +1326,74 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>16</v>
-      </c>
-      <c r="D7" t="s">
-        <v>17</v>
       </c>
       <c r="E7">
         <v>2018</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7">
-        <v>6216327</v>
+        <v>6216487</v>
       </c>
       <c r="H7">
-        <v>384865</v>
+        <v>385286</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E8">
         <v>2019</v>
       </c>
       <c r="F8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G8">
-        <v>6216327</v>
+        <v>6216487</v>
       </c>
       <c r="H8">
-        <v>384865</v>
+        <v>385286</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
-        <v>20</v>
+      <c r="C9">
+        <v>643</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E9">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="F9" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G9">
         <v>6216487</v>
@@ -1508,111 +1404,111 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10">
+        <v>2018</v>
+      </c>
+      <c r="F10" t="s">
         <v>21</v>
       </c>
-      <c r="E10">
-        <v>2019</v>
-      </c>
-      <c r="F10" t="s">
-        <v>22</v>
-      </c>
       <c r="G10">
-        <v>6216487</v>
+        <v>6216083</v>
       </c>
       <c r="H10">
-        <v>385286</v>
+        <v>384746</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="C11">
-        <v>643</v>
+      <c r="C11" t="s">
+        <v>22</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E11">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="F11" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G11">
-        <v>6216487</v>
+        <v>6216083</v>
       </c>
       <c r="H11">
-        <v>385286</v>
+        <v>384746</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3</v>
+        <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" t="s">
-        <v>24</v>
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>663</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E12">
-        <v>2018</v>
+        <v>2021</v>
       </c>
       <c r="F12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="G12">
-        <v>6216213</v>
+        <v>6216083</v>
       </c>
       <c r="H12">
-        <v>384673</v>
+        <v>384746</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" t="s">
         <v>27</v>
       </c>
-      <c r="D13" t="s">
-        <v>25</v>
-      </c>
       <c r="E13">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F13" t="s">
         <v>28</v>
       </c>
       <c r="G13">
-        <v>6216220</v>
+        <v>6216611</v>
       </c>
       <c r="H13">
-        <v>384664</v>
+        <v>384850</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -1621,71 +1517,71 @@
         <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E14">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="G14">
-        <v>6216083</v>
+        <v>6216611</v>
       </c>
       <c r="H14">
-        <v>384746</v>
+        <v>384850</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
       </c>
       <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15">
+        <v>2018</v>
+      </c>
+      <c r="F15" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
-        <v>30</v>
-      </c>
-      <c r="E15">
-        <v>2019</v>
-      </c>
-      <c r="F15" t="s">
-        <v>33</v>
-      </c>
       <c r="G15">
-        <v>6216083</v>
+        <v>6216622</v>
       </c>
       <c r="H15">
-        <v>384746</v>
+        <v>384283</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>43</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="C16">
-        <v>1023</v>
+      <c r="C16" t="s">
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E16">
-        <v>2021</v>
+        <v>2019</v>
       </c>
       <c r="F16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G16">
-        <v>6216083</v>
+        <v>6216622</v>
       </c>
       <c r="H16">
-        <v>384746</v>
+        <v>384283</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1693,103 +1589,103 @@
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1">
+        <v>666</v>
+      </c>
+      <c r="D17" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17">
+        <v>2021</v>
+      </c>
+      <c r="F17" t="s">
         <v>34</v>
       </c>
-      <c r="D17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E17">
-        <v>2018</v>
-      </c>
-      <c r="F17" t="s">
-        <v>36</v>
-      </c>
       <c r="G17">
-        <v>6216449</v>
+        <v>6216622</v>
       </c>
       <c r="H17">
-        <v>384330</v>
+        <v>384283</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18">
+        <v>2018</v>
+      </c>
+      <c r="F18" t="s">
         <v>37</v>
       </c>
-      <c r="D18" t="s">
-        <v>35</v>
-      </c>
-      <c r="E18">
-        <v>2019</v>
-      </c>
-      <c r="F18" t="s">
-        <v>36</v>
-      </c>
       <c r="G18">
-        <v>6216449</v>
+        <v>6216762</v>
       </c>
       <c r="H18">
-        <v>384330</v>
+        <v>384384</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
       </c>
       <c r="D19" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="E19">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="G19">
-        <v>6216444</v>
+        <v>6216762</v>
       </c>
       <c r="H19">
-        <v>384620</v>
+        <v>384384</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <v>2018</v>
+      </c>
+      <c r="F20" t="s">
         <v>41</v>
       </c>
-      <c r="D20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E20">
-        <v>2019</v>
-      </c>
-      <c r="F20" t="s">
-        <v>40</v>
-      </c>
       <c r="G20">
-        <v>6216444</v>
+        <v>6216787</v>
       </c>
       <c r="H20">
-        <v>384620</v>
+        <v>384588</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1797,143 +1693,143 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C21" t="s">
         <v>42</v>
       </c>
       <c r="D21" t="s">
+        <v>40</v>
+      </c>
+      <c r="E21">
+        <v>2019</v>
+      </c>
+      <c r="F21" t="s">
         <v>43</v>
       </c>
-      <c r="E21">
-        <v>2018</v>
-      </c>
-      <c r="F21" t="s">
-        <v>44</v>
-      </c>
       <c r="G21">
-        <v>6216306</v>
+        <v>6216787</v>
       </c>
       <c r="H21">
-        <v>384276</v>
+        <v>384588</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" t="s">
         <v>45</v>
       </c>
-      <c r="D22" t="s">
-        <v>43</v>
-      </c>
       <c r="E22">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F22" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="G22">
-        <v>6216293</v>
+        <v>6216853</v>
       </c>
       <c r="H22">
-        <v>384288</v>
+        <v>384271</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B23" t="s">
         <v>6</v>
       </c>
       <c r="C23" t="s">
+        <v>47</v>
+      </c>
+      <c r="D23" t="s">
+        <v>45</v>
+      </c>
+      <c r="E23">
+        <v>2019</v>
+      </c>
+      <c r="F23" t="s">
         <v>46</v>
       </c>
-      <c r="D23" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23">
-        <v>2018</v>
-      </c>
-      <c r="F23" t="s">
-        <v>48</v>
-      </c>
       <c r="G23">
-        <v>6216611</v>
+        <v>6216853</v>
       </c>
       <c r="H23">
-        <v>384850</v>
+        <v>384271</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
         <v>6</v>
       </c>
-      <c r="C24" t="s">
-        <v>49</v>
+      <c r="C24" s="1">
+        <v>659</v>
       </c>
       <c r="D24" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E24">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="F24" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G24">
-        <v>6216611</v>
+        <v>6216853</v>
       </c>
       <c r="H24">
-        <v>384850</v>
+        <v>384271</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C25" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" t="s">
         <v>50</v>
-      </c>
-      <c r="D25" t="s">
-        <v>51</v>
       </c>
       <c r="E25">
         <v>2018</v>
       </c>
       <c r="F25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G25">
-        <v>6216680</v>
+        <v>6217218</v>
       </c>
       <c r="H25">
-        <v>384632</v>
+        <v>384600</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="D26" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E26">
         <v>2019</v>
@@ -1942,62 +1838,62 @@
         <v>52</v>
       </c>
       <c r="G26">
-        <v>6216680</v>
+        <v>6217218</v>
       </c>
       <c r="H26">
-        <v>384632</v>
+        <v>384600</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>29</v>
+        <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C27" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E27">
         <v>2018</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G27">
-        <v>6216631</v>
+        <v>6217150</v>
       </c>
       <c r="H27">
-        <v>384393</v>
+        <v>384900</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>19</v>
+        <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E28">
         <v>2019</v>
       </c>
       <c r="F28" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="G28">
-        <v>6216631</v>
+        <v>6217150</v>
       </c>
       <c r="H28">
-        <v>384393</v>
+        <v>384900</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -2005,103 +1901,103 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C29" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D29" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E29">
         <v>2018</v>
       </c>
       <c r="F29" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G29">
-        <v>6216622</v>
+        <v>6217161</v>
       </c>
       <c r="H29">
-        <v>384283</v>
+        <v>384771</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C30" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="D30" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E30">
         <v>2019</v>
       </c>
       <c r="F30" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="G30">
-        <v>6216622</v>
+        <v>6217161</v>
       </c>
       <c r="H30">
-        <v>384283</v>
+        <v>384771</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
-      </c>
-      <c r="C31">
-        <v>1026</v>
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
+        <v>25</v>
       </c>
       <c r="D31" t="s">
         <v>59</v>
       </c>
       <c r="E31">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="F31" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G31">
-        <v>6216622</v>
+        <v>6217114</v>
       </c>
       <c r="H31">
-        <v>384283</v>
+        <v>384764</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C32" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D32" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="E32">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F32" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="G32">
-        <v>6216762</v>
+        <v>6217114</v>
       </c>
       <c r="H32">
-        <v>384384</v>
+        <v>384764</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -2112,126 +2008,126 @@
         <v>6</v>
       </c>
       <c r="C33" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D33" t="s">
+        <v>63</v>
+      </c>
+      <c r="E33">
+        <v>2018</v>
+      </c>
+      <c r="F33" t="s">
         <v>64</v>
       </c>
-      <c r="E33">
-        <v>2019</v>
-      </c>
-      <c r="F33" t="s">
-        <v>65</v>
-      </c>
       <c r="G33">
-        <v>6216762</v>
+        <v>6217007</v>
       </c>
       <c r="H33">
-        <v>384384</v>
+        <v>384180</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B34" t="s">
         <v>6</v>
       </c>
       <c r="C34" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D34" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E34">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F34" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G34">
-        <v>6216787</v>
+        <v>6217007</v>
       </c>
       <c r="H34">
-        <v>384588</v>
+        <v>384180</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B35" t="s">
         <v>6</v>
       </c>
-      <c r="C35" t="s">
-        <v>70</v>
+      <c r="C35" s="1">
+        <v>659</v>
       </c>
       <c r="D35" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="E35">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="F35" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="G35">
-        <v>6216787</v>
+        <v>6217007</v>
       </c>
       <c r="H35">
-        <v>384588</v>
+        <v>384180</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B36" t="s">
         <v>6</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="D36" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E36">
         <v>2018</v>
       </c>
       <c r="F36" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G36">
-        <v>6216853</v>
+        <v>6216991</v>
       </c>
       <c r="H36">
-        <v>384271</v>
+        <v>384214</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B37" t="s">
         <v>6</v>
       </c>
       <c r="C37" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D37" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E37">
         <v>2019</v>
       </c>
       <c r="F37" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="G37">
-        <v>6216853</v>
+        <v>6216991</v>
       </c>
       <c r="H37">
-        <v>384271</v>
+        <v>384214</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
@@ -2241,49 +2137,49 @@
       <c r="B38" t="s">
         <v>6</v>
       </c>
-      <c r="C38">
-        <v>1028</v>
+      <c r="C38" t="s">
+        <v>70</v>
       </c>
       <c r="D38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E38">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="F38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G38">
-        <v>6216853</v>
+        <v>6217085</v>
       </c>
       <c r="H38">
-        <v>384271</v>
+        <v>384230</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B39" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="C39" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D39" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="E39">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F39" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="G39">
-        <v>6217218</v>
+        <v>6217085</v>
       </c>
       <c r="H39">
-        <v>384600</v>
+        <v>384230</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
@@ -2291,25 +2187,25 @@
         <v>0</v>
       </c>
       <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
+        <v>74</v>
+      </c>
+      <c r="D40" t="s">
+        <v>75</v>
+      </c>
+      <c r="E40">
+        <v>2018</v>
+      </c>
+      <c r="F40" t="s">
         <v>76</v>
       </c>
-      <c r="C40" t="s">
-        <v>70</v>
-      </c>
-      <c r="D40" t="s">
-        <v>78</v>
-      </c>
-      <c r="E40">
-        <v>2019</v>
-      </c>
-      <c r="F40" t="s">
-        <v>80</v>
-      </c>
       <c r="G40">
-        <v>6217218</v>
+        <v>6217140</v>
       </c>
       <c r="H40">
-        <v>384600</v>
+        <v>384408</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
@@ -2317,25 +2213,25 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" t="s">
+        <v>77</v>
+      </c>
+      <c r="D41" t="s">
+        <v>75</v>
+      </c>
+      <c r="E41">
+        <v>2019</v>
+      </c>
+      <c r="F41" t="s">
         <v>76</v>
       </c>
-      <c r="C41" t="s">
-        <v>38</v>
-      </c>
-      <c r="D41" t="s">
-        <v>81</v>
-      </c>
-      <c r="E41">
-        <v>2018</v>
-      </c>
-      <c r="F41" t="s">
-        <v>82</v>
-      </c>
       <c r="G41">
-        <v>6217150</v>
+        <v>6217140</v>
       </c>
       <c r="H41">
-        <v>384900</v>
+        <v>384408</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
@@ -2343,25 +2239,25 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C42" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D42" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E42">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F42" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G42">
-        <v>6217150</v>
+        <v>6217647</v>
       </c>
       <c r="H42">
-        <v>384900</v>
+        <v>384510</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
@@ -2369,337 +2265,337 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D43" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E43">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F43" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G43">
-        <v>6217161</v>
+        <v>6217647</v>
       </c>
       <c r="H43">
-        <v>384771</v>
+        <v>384510</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B44" t="s">
-        <v>76</v>
-      </c>
-      <c r="C44" t="s">
-        <v>70</v>
+        <v>48</v>
+      </c>
+      <c r="C44">
+        <v>659</v>
       </c>
       <c r="D44" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="E44">
-        <v>2019</v>
+        <v>2021</v>
       </c>
       <c r="F44" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="G44">
-        <v>6217161</v>
+        <v>6217647</v>
       </c>
       <c r="H44">
-        <v>384771</v>
+        <v>384510</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C45" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="D45" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E45">
         <v>2018</v>
       </c>
       <c r="F45" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G45">
-        <v>6217114</v>
+        <v>6217417</v>
       </c>
       <c r="H45">
-        <v>384764</v>
+        <v>384722</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="C46" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D46" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E46">
         <v>2019</v>
       </c>
       <c r="F46" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G46">
-        <v>6217114</v>
+        <v>6217417</v>
       </c>
       <c r="H46">
-        <v>384764</v>
+        <v>384722</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B47" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C47" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D47" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E47">
         <v>2018</v>
       </c>
       <c r="F47" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G47">
-        <v>6217007</v>
+        <v>6217568</v>
       </c>
       <c r="H47">
-        <v>384180</v>
+        <v>384846</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C48" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="D48" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E48">
         <v>2019</v>
       </c>
       <c r="F48" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G48">
-        <v>6217007</v>
+        <v>6217568</v>
       </c>
       <c r="H48">
-        <v>384180</v>
+        <v>384846</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="C49">
-        <v>1019</v>
+        <v>629</v>
       </c>
       <c r="D49" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E49">
         <v>2021</v>
       </c>
       <c r="F49" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="G49">
-        <v>6217007</v>
+        <v>6217568</v>
       </c>
       <c r="H49">
-        <v>384180</v>
+        <v>384846</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B50" t="s">
         <v>6</v>
       </c>
       <c r="C50" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D50" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E50">
         <v>2018</v>
       </c>
       <c r="F50" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G50">
-        <v>6216991</v>
+        <v>6217559</v>
       </c>
       <c r="H50">
-        <v>384214</v>
+        <v>385005</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B51" t="s">
         <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>97</v>
+        <v>22</v>
       </c>
       <c r="D51" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E51">
         <v>2019</v>
       </c>
       <c r="F51" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G51">
-        <v>6216991</v>
+        <v>6217559</v>
       </c>
       <c r="H51">
-        <v>384214</v>
+        <v>385005</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="B52" t="s">
         <v>6</v>
       </c>
       <c r="C52" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D52" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E52">
         <v>2018</v>
       </c>
       <c r="F52" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G52">
-        <v>6217085</v>
+        <v>6217491</v>
       </c>
       <c r="H52">
-        <v>384230</v>
+        <v>385037</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B53" t="s">
         <v>6</v>
       </c>
       <c r="C53" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D53" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E53">
         <v>2019</v>
       </c>
       <c r="F53" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="G53">
-        <v>6217085</v>
+        <v>6217491</v>
       </c>
       <c r="H53">
-        <v>384230</v>
+        <v>385037</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B54" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="C54" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D54" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E54">
         <v>2018</v>
       </c>
       <c r="F54" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G54">
-        <v>6217140</v>
+        <v>6216919</v>
       </c>
       <c r="H54">
-        <v>384408</v>
+        <v>384957</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D55" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="E55">
         <v>2019</v>
       </c>
       <c r="F55" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G55">
-        <v>6217140</v>
+        <v>6216919</v>
       </c>
       <c r="H55">
-        <v>384408</v>
+        <v>384957</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -2707,571 +2603,103 @@
         <v>0</v>
       </c>
       <c r="B56" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="C56" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D56" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E56">
         <v>2018</v>
       </c>
       <c r="F56" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G56">
-        <v>6217647</v>
+        <v>6217025</v>
       </c>
       <c r="H56">
-        <v>384510</v>
+        <v>385133</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D57" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E57">
         <v>2019</v>
       </c>
       <c r="F57" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="G57">
-        <v>6217647</v>
+        <v>6217025</v>
       </c>
       <c r="H57">
-        <v>384510</v>
+        <v>385133</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>76</v>
-      </c>
-      <c r="C58">
-        <v>808</v>
+        <v>6</v>
+      </c>
+      <c r="C58" t="s">
+        <v>93</v>
       </c>
       <c r="D58" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E58">
-        <v>2021</v>
+        <v>2018</v>
       </c>
       <c r="F58" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G58">
-        <v>6217647</v>
+        <v>6216394</v>
       </c>
       <c r="H58">
-        <v>384510</v>
+        <v>384921</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B59" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="C59" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D59" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="E59">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F59" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="G59">
-        <v>6217417</v>
+        <v>6216394</v>
       </c>
       <c r="H59">
-        <v>384722</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>0</v>
-      </c>
-      <c r="B60" t="s">
-        <v>76</v>
-      </c>
-      <c r="C60" t="s">
-        <v>113</v>
-      </c>
-      <c r="D60" t="s">
-        <v>111</v>
-      </c>
-      <c r="E60">
-        <v>2019</v>
-      </c>
-      <c r="F60" t="s">
-        <v>112</v>
-      </c>
-      <c r="G60">
-        <v>6217417</v>
-      </c>
-      <c r="H60">
-        <v>384722</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>2</v>
-      </c>
-      <c r="B61" t="s">
-        <v>76</v>
-      </c>
-      <c r="C61" t="s">
-        <v>114</v>
-      </c>
-      <c r="D61" t="s">
-        <v>115</v>
-      </c>
-      <c r="E61">
-        <v>2018</v>
-      </c>
-      <c r="F61" t="s">
-        <v>116</v>
-      </c>
-      <c r="G61">
-        <v>6217568</v>
-      </c>
-      <c r="H61">
-        <v>384846</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>3</v>
-      </c>
-      <c r="B62" t="s">
-        <v>76</v>
-      </c>
-      <c r="C62" t="s">
-        <v>117</v>
-      </c>
-      <c r="D62" t="s">
-        <v>115</v>
-      </c>
-      <c r="E62">
-        <v>2019</v>
-      </c>
-      <c r="F62" t="s">
-        <v>116</v>
-      </c>
-      <c r="G62">
-        <v>6217568</v>
-      </c>
-      <c r="H62">
-        <v>384846</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>0</v>
-      </c>
-      <c r="B63" t="s">
-        <v>76</v>
-      </c>
-      <c r="C63">
-        <v>629</v>
-      </c>
-      <c r="D63" t="s">
-        <v>115</v>
-      </c>
-      <c r="E63">
-        <v>2021</v>
-      </c>
-      <c r="F63" t="s">
-        <v>116</v>
-      </c>
-      <c r="G63">
-        <v>6217568</v>
-      </c>
-      <c r="H63">
-        <v>384846</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>0</v>
-      </c>
-      <c r="B64" t="s">
-        <v>6</v>
-      </c>
-      <c r="C64" t="s">
-        <v>118</v>
-      </c>
-      <c r="D64" t="s">
-        <v>119</v>
-      </c>
-      <c r="E64">
-        <v>2018</v>
-      </c>
-      <c r="F64" t="s">
-        <v>120</v>
-      </c>
-      <c r="G64">
-        <v>6217559</v>
-      </c>
-      <c r="H64">
-        <v>385005</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>1</v>
-      </c>
-      <c r="B65" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65" t="s">
-        <v>32</v>
-      </c>
-      <c r="D65" t="s">
-        <v>119</v>
-      </c>
-      <c r="E65">
-        <v>2019</v>
-      </c>
-      <c r="F65" t="s">
-        <v>120</v>
-      </c>
-      <c r="G65">
-        <v>6217559</v>
-      </c>
-      <c r="H65">
-        <v>385005</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>0</v>
-      </c>
-      <c r="B66" t="s">
-        <v>6</v>
-      </c>
-      <c r="C66" t="s">
-        <v>121</v>
-      </c>
-      <c r="D66" t="s">
-        <v>122</v>
-      </c>
-      <c r="E66">
-        <v>2018</v>
-      </c>
-      <c r="F66" t="s">
-        <v>123</v>
-      </c>
-      <c r="G66">
-        <v>6217491</v>
-      </c>
-      <c r="H66">
-        <v>385037</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>0</v>
-      </c>
-      <c r="B67" t="s">
-        <v>6</v>
-      </c>
-      <c r="C67" t="s">
-        <v>124</v>
-      </c>
-      <c r="D67" t="s">
-        <v>122</v>
-      </c>
-      <c r="E67">
-        <v>2019</v>
-      </c>
-      <c r="F67" t="s">
-        <v>123</v>
-      </c>
-      <c r="G67">
-        <v>6217491</v>
-      </c>
-      <c r="H67">
-        <v>385037</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>1</v>
-      </c>
-      <c r="B68" t="s">
-        <v>6</v>
-      </c>
-      <c r="C68" t="s">
-        <v>125</v>
-      </c>
-      <c r="D68" t="s">
-        <v>126</v>
-      </c>
-      <c r="E68">
-        <v>2018</v>
-      </c>
-      <c r="F68" t="s">
-        <v>127</v>
-      </c>
-      <c r="G68">
-        <v>6216919</v>
-      </c>
-      <c r="H68">
-        <v>384957</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>2</v>
-      </c>
-      <c r="B69" t="s">
-        <v>6</v>
-      </c>
-      <c r="C69" t="s">
-        <v>128</v>
-      </c>
-      <c r="D69" t="s">
-        <v>126</v>
-      </c>
-      <c r="E69">
-        <v>2019</v>
-      </c>
-      <c r="F69" t="s">
-        <v>127</v>
-      </c>
-      <c r="G69">
-        <v>6216919</v>
-      </c>
-      <c r="H69">
-        <v>384957</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70">
-        <v>0</v>
-      </c>
-      <c r="B70" t="s">
-        <v>6</v>
-      </c>
-      <c r="C70" t="s">
-        <v>129</v>
-      </c>
-      <c r="D70" t="s">
-        <v>130</v>
-      </c>
-      <c r="E70">
-        <v>2018</v>
-      </c>
-      <c r="F70" t="s">
-        <v>131</v>
-      </c>
-      <c r="G70">
-        <v>6217025</v>
-      </c>
-      <c r="H70">
-        <v>385133</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>2</v>
-      </c>
-      <c r="B71" t="s">
-        <v>6</v>
-      </c>
-      <c r="C71" t="s">
-        <v>132</v>
-      </c>
-      <c r="D71" t="s">
-        <v>130</v>
-      </c>
-      <c r="E71">
-        <v>2019</v>
-      </c>
-      <c r="F71" t="s">
-        <v>131</v>
-      </c>
-      <c r="G71">
-        <v>6217025</v>
-      </c>
-      <c r="H71">
-        <v>385133</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72">
-        <v>3</v>
-      </c>
-      <c r="B72" t="s">
-        <v>6</v>
-      </c>
-      <c r="C72" t="s">
-        <v>121</v>
-      </c>
-      <c r="D72" t="s">
-        <v>133</v>
-      </c>
-      <c r="E72">
-        <v>2018</v>
-      </c>
-      <c r="F72" t="s">
-        <v>134</v>
-      </c>
-      <c r="G72">
-        <v>6216394</v>
-      </c>
-      <c r="H72">
         <v>384921</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73">
-        <v>1</v>
-      </c>
-      <c r="B73" t="s">
-        <v>6</v>
-      </c>
-      <c r="C73" t="s">
-        <v>135</v>
-      </c>
-      <c r="D73" t="s">
-        <v>133</v>
-      </c>
-      <c r="E73">
-        <v>2019</v>
-      </c>
-      <c r="F73" t="s">
-        <v>134</v>
-      </c>
-      <c r="G73">
-        <v>6216394</v>
-      </c>
-      <c r="H73">
-        <v>384921</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74">
-        <v>128</v>
-      </c>
-      <c r="B74" t="s">
-        <v>15</v>
-      </c>
-      <c r="C74" t="s">
-        <v>136</v>
-      </c>
-      <c r="D74" t="s">
-        <v>137</v>
-      </c>
-      <c r="E74">
-        <v>2018</v>
-      </c>
-      <c r="F74" t="s">
-        <v>138</v>
-      </c>
-      <c r="G74">
-        <v>6216342</v>
-      </c>
-      <c r="H74">
-        <v>384334</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75">
-        <v>659</v>
-      </c>
-      <c r="B75" t="s">
-        <v>15</v>
-      </c>
-      <c r="C75" t="s">
-        <v>97</v>
-      </c>
-      <c r="D75" t="s">
-        <v>137</v>
-      </c>
-      <c r="E75">
-        <v>2019</v>
-      </c>
-      <c r="F75" t="s">
-        <v>138</v>
-      </c>
-      <c r="G75">
-        <v>6216342</v>
-      </c>
-      <c r="H75">
-        <v>384334</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76">
-        <v>72</v>
-      </c>
-      <c r="B76" t="s">
-        <v>15</v>
-      </c>
-      <c r="C76" t="s">
-        <v>139</v>
-      </c>
-      <c r="D76" t="s">
-        <v>140</v>
-      </c>
-      <c r="E76">
-        <v>2018</v>
-      </c>
-      <c r="F76" t="s">
-        <v>141</v>
-      </c>
-      <c r="G76">
-        <v>6216318</v>
-      </c>
-      <c r="H76">
-        <v>384497</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77">
-        <v>208</v>
-      </c>
-      <c r="B77" t="s">
-        <v>15</v>
-      </c>
-      <c r="C77" t="s">
-        <v>142</v>
-      </c>
-      <c r="D77" t="s">
-        <v>140</v>
-      </c>
-      <c r="E77">
-        <v>2019</v>
-      </c>
-      <c r="F77" t="s">
-        <v>141</v>
-      </c>
-      <c r="G77">
-        <v>6216318</v>
-      </c>
-      <c r="H77">
-        <v>384497</v>
       </c>
     </row>
   </sheetData>

</xml_diff>